<commit_message>
gov rev update, grants update, fix n/a in gdp, and user data
</commit_message>
<xml_diff>
--- a/user-data/ethiopia-nigeria-r3/ethiopia-nigeria-r3.xlsx
+++ b/user-data/ethiopia-nigeria-r3/ethiopia-nigeria-r3.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Data-wide-value" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +151,12 @@
     <t>Nigeria</t>
   </si>
   <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
     <t>Name: ethiopia-nigeria-r3</t>
   </si>
   <si>
@@ -166,6 +173,9 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>On the 'Data-wide-value' sheet, we have provided the indicator in a wide format. The values you see listed there are from the 'value' column.</t>
   </si>
   <si>
     <t>The following is data downloaded from Development Initiative's Datahub: http://devinit.org/data</t>
@@ -514,47 +524,47 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -564,22 +574,32 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1976,4 +1996,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3359031639</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3565493249</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2545783781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>